<commit_message>
Plan de charge automatisé
</commit_message>
<xml_diff>
--- a/1 - Avant Projet/1 - Échanges/6 - Plan de charges.xlsx
+++ b/1 - Avant Projet/1 - Échanges/6 - Plan de charges.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom Grandjean\Documents\SeriousGame\Serious-Game-MMI\1 - Avant Projet\1 - Échanges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C58D465-6E1D-48E8-92BC-01CF04CB3A1C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B4A069-A999-4808-B620-4310E7BD7AD8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9636" xr2:uid="{16F4FCEC-5E8F-4D04-A879-F6C6C49C782F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Étapes</t>
   </si>
@@ -45,22 +45,24 @@
     <t>Étude logiciels</t>
   </si>
   <si>
-    <t>1h</t>
-  </si>
-  <si>
-    <t>2h</t>
-  </si>
-  <si>
-    <t>0,5h</t>
-  </si>
-  <si>
-    <t>Arborescence</t>
+    <t>COÛT Horaire</t>
+  </si>
+  <si>
+    <t>COÛT Total</t>
+  </si>
+  <si>
+    <t>Mise en route</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0\ &quot;€&quot;"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -90,13 +92,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -107,6 +125,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FBEC4B69-9585-4D2D-9A7D-9AC031522D06}" name="Tableau3" displayName="Tableau3" ref="A1:E3" totalsRowShown="0">
+  <autoFilter ref="A1:E3" xr:uid="{714E2B9A-5FFA-4192-B4EF-396AF1B7C974}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{75AB691D-3757-4E23-BF2C-1BAE3B4FECC6}" name="Étapes"/>
+    <tableColumn id="2" xr3:uid="{AD45AE14-2BCC-4EF4-8DC0-84749876A72A}" name="Nb d'h Tom" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{ABE271CE-17E9-4BF1-95F7-9DACA5A45BD5}" name="Nb d'h Loïc" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{86AACC64-F1E5-4A04-85BF-7DF0A30DC284}" name="Nb d'h Anuar" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{866254C7-8BAB-4B5D-9916-6044FCF3926F}" name="Nb d'h M. KARINE" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -406,17 +438,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EEE36C8-0380-4082-956B-364ACD7E47C0}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -440,33 +472,77 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
+      <c r="B13" s="3">
+        <f>SUM(Tableau3[Nb d''h Tom])*B12</f>
+        <v>90</v>
+      </c>
+      <c r="C13" s="3">
+        <f>SUM(Tableau3[Nb d''h Loïc])*C12</f>
+        <v>20</v>
+      </c>
+      <c r="D13" s="3">
+        <f>SUM(Tableau3[Nb d''h Anuar])*D12</f>
+        <v>30</v>
+      </c>
+      <c r="E13" s="3">
+        <f>SUM(Tableau3[Nb d''h M. KARINE])*E12</f>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MàJ Plan de charge AP
</commit_message>
<xml_diff>
--- a/1 - Avant Projet/1 - Échanges/6 - Plan de charges.xlsx
+++ b/1 - Avant Projet/1 - Échanges/6 - Plan de charges.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom Grandjean\Documents\SeriousGame\Serious-Game-MMI\1 - Avant Projet\1 - Échanges\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Serious-Game-MMI\1 - Avant Projet\1 - Échanges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAD0369-787A-4160-A61F-41D90D69EA65}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DA254D40-0E8E-4A85-9E5A-65AFDA3575F4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9636" xr2:uid="{16F4FCEC-5E8F-4D04-A879-F6C6C49C782F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9630" xr2:uid="{16F4FCEC-5E8F-4D04-A879-F6C6C49C782F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -447,19 +447,19 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,12 +476,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="C2" s="2">
         <v>0.5</v>
@@ -493,7 +493,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -510,7 +510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -523,7 +523,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -540,13 +540,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="3">
         <f>SUM(Tableau3[Tom])*B12</f>
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="C13" s="3">
         <f>SUM(Tableau3[Loïc])*C12</f>
@@ -561,13 +561,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
       <c r="B15">
         <f>SUM(Tableau3[[Tom]:[Nb d''h M. KARINE]])</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualisation plan de charges
</commit_message>
<xml_diff>
--- a/1 - Avant Projet/1 - Échanges/6 - Plan de charges.xlsx
+++ b/1 - Avant Projet/1 - Échanges/6 - Plan de charges.xlsx
@@ -446,7 +446,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,8 +454,8 @@
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -483,10 +483,10 @@
         <v>4.5</v>
       </c>
       <c r="C2" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E2" s="2">
         <v>0.5</v>
@@ -549,11 +549,11 @@
       </c>
       <c r="C13" s="3">
         <f>SUM(Tableau3[Loïc])*C12</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D13" s="3">
         <f>SUM(Tableau3[Anuar])*D12</f>
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E13" s="3">
         <f>SUM(Tableau3[Nb d''h M. KARINE])*E12</f>
@@ -566,7 +566,7 @@
       </c>
       <c r="B15">
         <f>SUM(Tableau3[[Tom]:[Nb d''h M. KARINE]])</f>
-        <v>16.5</v>
+        <v>17.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>